<commit_message>
Re-run inventory parse and Excel with case logic
</commit_message>
<xml_diff>
--- a/mise_inventory/113025_inventory_final.xlsx
+++ b/mise_inventory/113025_inventory_final.xlsx
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>75.5</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10">
@@ -668,7 +668,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5">
@@ -688,7 +688,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>14</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
Inventory: add deps and regenerate 113025 output
</commit_message>
<xml_diff>
--- a/mise_inventory/113025_inventory_final.xlsx
+++ b/mise_inventory/113025_inventory_final.xlsx
@@ -12,6 +12,8 @@
     <sheet name="Wine Cost" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Liquor Cost" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="N-A Beverage Cost" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="grocery__dry_goods" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="na_beverage" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,6 +431,24 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -452,11 +472,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Tajin Seasoning</t>
+          <t>Grayton 30A Beach Blonde Keg</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -464,264 +484,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Item</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Athletic Upside Dawn NA (cans)</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Coors Light (cans)</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Grayton 30A Beach Blonde Keg</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Grayton Gose (cans)</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>High Noon (cans)</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>High Rise Pineapple THC Seltzer (cans)</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Kona Big Wave Keg</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Michelob Ultra (cans)</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Miller Lite (cans)</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Mom Water (cans)</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Urban South Paradise Park Keg (1/6BBL)</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Yuengling (cans)</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Item</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>30A Cabernet Sauvignon</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>30A Chardonnay</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>30A Rosé</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>30A Sauvignon Blanc</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Canoe Ridge Merlot</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Scarpetta Pinot Grigio</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>The Shaker Red Blend</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Windstorm Chardonnay</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -760,4 +536,40 @@
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Inventory: disable default normalization and fix parser robustness
</commit_message>
<xml_diff>
--- a/mise_inventory/113025_inventory_final.xlsx
+++ b/mise_inventory/113025_inventory_final.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,11 +472,141 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Athletic Upside Dawn Golden 12oz Can</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Athletic Upside Dawn NA (cans)</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Coors Light 12oz Can</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Fairhope I Drink Therefore I Amber Keg</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>914.25</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>Grayton 30A Beach Blonde Keg</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>95</v>
+      <c r="B6" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Grayton Beach 30A Rosé 12oz Can</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>High Noon (cans)</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>High Rise Blood Orange 12oz Can</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>High Rise Pineapple THC Seltzer (cans)</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Michelob Ultra (cans)</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Miller Lite (cans)</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Miller Lite 12oz Can</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>205.5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Mom Water Linda 12oz Can</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>57.5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Yuengling (cans)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -490,14 +620,47 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Item</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Carter's Lot Rosé of Pinot Noir 750ml</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>The Shaker Red Blend</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add location-aware breakdown to parser and Excel
</commit_message>
<xml_diff>
--- a/mise_inventory/113025_inventory_final.xlsx
+++ b/mise_inventory/113025_inventory_final.xlsx
@@ -701,7 +701,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D188"/>
+  <dimension ref="A1:E188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -730,6 +730,11 @@
           <t>Source</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -750,6 +755,11 @@
           <t>85 percent of a bottle of tia maria espresso coffee liqueur</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>back bar</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -770,6 +780,11 @@
           <t>walnut liqueur three quarters of a bottle of ferretti espresso coffee liqueur two point eight bottles of campari</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -787,7 +802,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>16 cans of Miller Lite</t>
+          <t>16 one bottle of Blue Agave</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -803,11 +823,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1 bottle of Bloody Mary Mix</t>
+          <t>13 cans of high rise pineapple</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -823,11 +848,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1 bottle of</t>
+          <t>16 cans of Miller Lite</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -847,7 +877,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1 bottle of 30a Chardonnay</t>
+          <t>1 bottle of Bloody Mary Mix</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -867,7 +902,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1 bottle of Windstorm Chardonnay</t>
+          <t>1 bottle of</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -883,11 +923,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>16 one bottle of Blue Agave</t>
+          <t>1 bottle of 30a Chardonnay</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -903,11 +948,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>13 cans of high rise pineapple</t>
+          <t>1 bottle of Windstorm Chardonnay</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -930,6 +980,11 @@
           <t>13 bottles of canoe ridge merlot</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -950,6 +1005,11 @@
           <t>11 bottles of cream of coconut</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -970,6 +1030,11 @@
           <t>14 bottles of grenadine</t>
         </is>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -990,6 +1055,11 @@
           <t>16 bottles of tahini</t>
         </is>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1010,6 +1080,11 @@
           <t>11 bottles of siete misterios mezcal</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1030,6 +1105,11 @@
           <t>11 bottles of milagros silver</t>
         </is>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1050,6 +1130,11 @@
           <t>11 bottles of meyers original dark rum</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1063,11 +1148,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.9</v>
+        <v>24</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>of Redwood Empire 90% of a bottle of Nickters 75% of a bottle of the shaker red blend full</t>
+          <t>24 Coors lights 13 athletic non-alcoholic beers</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -1083,11 +1173,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.8</v>
+        <v>10</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>bottle of canoe Ridge Merlot 80% of a bottle of windstorm Chardonnay 75% of a bottle of Campari</t>
+          <t>10 Yinglings</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -1103,11 +1198,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.8</v>
+        <v>14</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>a full bottle of Campesino aged rum 80% of a bottle of Campesino silver rum 95% of a bottle</t>
+          <t>14 Pacificos 24 Michelob Ultras</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -1123,11 +1223,16 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.8</v>
+        <v>24</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>of Jack Daniel's 80% of a bottle of Myers aged rum full bottle of sham board 75% of a bottle of</t>
+          <t>24 pack of micolob ultra</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -1143,11 +1248,16 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>and this bottle is 750 milliliters full bottle of crop lemon full bottle of Parrot Bay coconut</t>
+          <t>24 pack of yingling</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -1163,11 +1273,16 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.75</v>
+        <v>12</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Bay coconut rum half of a bottle of Parrot Bay white rum 75% of a bottle of Yahweh 90% of a bottle</t>
+          <t>12 pack of miller light</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -1183,11 +1298,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.25</v>
+        <v>12</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>of Siete Mesterios mezcal 25% of a bottle of Pueblo Viejo 20% of a bottle of triple sec</t>
+          <t>12 pack of pacifico</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -1203,11 +1323,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>count as well in storage we have a full 12 bottle case of Wheatley's so let's add that to the count</t>
+          <t>12 pack of coarse light full bottle of jack daniels</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -1223,11 +1348,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>22</v>
+        <v>0.5</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>22 cans of Yingling</t>
+          <t>a half bottles of parrot bay coconut rum full bottle of wheatleys full 750 milliliter</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -1243,11 +1373,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>5 cans of athletic non-alcoholic beer</t>
+          <t>75 bottles of jim beam full bottle of makers mark full bottle of milagro reposado</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -1263,11 +1398,16 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>12</v>
+        <v>0.1</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>12 cans of Coors Light</t>
+          <t>10 percent of a bottle of rumple mints 25 percent of a bottle of jagermeister</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -1283,11 +1423,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>24</v>
+        <v>0.75</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>24 cans of high noon</t>
+          <t>75 percent of a bottle of rumple mints full bottle of jalapeno simple syrup</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -1303,11 +1448,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>2</v>
+        <v>0.75</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2 bottles of Squealing Pig</t>
+          <t>75 percent of a bottle of romano romana amaro full bottle of hendrix gin</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -1323,11 +1473,16 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>half of a bottle of Pueblo Viejo 90% of a bottle of Yahweh 25% of a bottle of Eagle</t>
+          <t>walnut liqueur 85 percent of a bottle of tulamore dew 25 percent of a bottle of</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -1343,11 +1498,16 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.5</v>
+        <v>24</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Rare 10 year aged quarter of a bottle of E.H. Taylor half of a bottle of Parrot Bay white rum</t>
+          <t>24 cans of myckelope ultra</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -1363,11 +1523,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.5</v>
+        <v>13</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>then a half of a 750 milliliter bottle of</t>
+          <t>13 cans of greaton 30a gosey 24 more cans of myckelope ultra</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -1383,11 +1548,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.2</v>
+        <v>12</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Grey Goose 20% of a bottle of Woodford half of a bottle of Jim Beam a full bottle of Mikters 80%</t>
+          <t>12 pack of pacifico two</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -1403,11 +1573,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.25</v>
+        <v>12</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>of a bottle of Crown 25% of a bottle of Hendrick's Gin 90% of a bottle of Casamigos 25% of a bottle</t>
+          <t>12 cans of yingling</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -1423,11 +1598,16 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.85</v>
+        <v>20</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>of Milagro Reposado a full bottle of Milagro Silver 85% of a bottle of Blanton's 80% of a bottle</t>
+          <t>20 cans of mom water got a high noon</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -1443,11 +1623,16 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.98</v>
+        <v>0.75</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>of Caravella 98% of a bottle of Maker's Mark 80% of a bottle of Grand Gala 95% of a bottle</t>
+          <t>full bottle of canoe ridge 75 percent of a bottle of canoe ridge full bottle of</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -1463,11 +1648,16 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.1</v>
+        <v>144</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>of Bowles elderflower liqueur half of a bottle of Blue Curacao 10% of a bottle of Jack Daniels</t>
+          <t>12 bottle cases of 30a rose</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -1483,11 +1673,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>24</v>
+        <v>144</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>24 Coors lights 13 athletic non-alcoholic beers</t>
+          <t>12 bottle cases of 30a</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -1503,11 +1698,16 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>10</v>
+        <v>0.9</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>10 Yinglings</t>
+          <t>of Redwood Empire 90% of a bottle of Nickters 75% of a bottle of the shaker red blend full</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>inside bar</t>
         </is>
       </c>
     </row>
@@ -1523,11 +1723,16 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>14</v>
+        <v>0.8</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>14 Pacificos 24 Michelob Ultras</t>
+          <t>bottle of canoe Ridge Merlot 80% of a bottle of windstorm Chardonnay 75% of a bottle of Campari</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>inside bar</t>
         </is>
       </c>
     </row>
@@ -1543,11 +1748,16 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>24</v>
+        <v>0.8</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>24 pack of micolob ultra</t>
+          <t>a full bottle of Campesino aged rum 80% of a bottle of Campesino silver rum 95% of a bottle</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>inside bar</t>
         </is>
       </c>
     </row>
@@ -1563,11 +1773,16 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>24</v>
+        <v>0.8</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>24 pack of yingling</t>
+          <t>of Jack Daniel's 80% of a bottle of Myers aged rum full bottle of sham board 75% of a bottle of</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>inside bar</t>
         </is>
       </c>
     </row>
@@ -1583,11 +1798,16 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>12 pack of miller light</t>
+          <t>and this bottle is 750 milliliters full bottle of crop lemon full bottle of Parrot Bay coconut</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>inside bar</t>
         </is>
       </c>
     </row>
@@ -1603,11 +1823,16 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>12</v>
+        <v>0.75</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>12 pack of pacifico</t>
+          <t>Bay coconut rum half of a bottle of Parrot Bay white rum 75% of a bottle of Yahweh 90% of a bottle</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>inside bar</t>
         </is>
       </c>
     </row>
@@ -1623,11 +1848,16 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>12 pack of coarse light full bottle of jack daniels</t>
+          <t>of Siete Mesterios mezcal 25% of a bottle of Pueblo Viejo 20% of a bottle of triple sec</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>inside bar</t>
         </is>
       </c>
     </row>
@@ -1643,11 +1873,16 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.5</v>
+        <v>12</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>a half bottles of parrot bay coconut rum full bottle of wheatleys full 750 milliliter</t>
+          <t>count as well in storage we have a full 12 bottle case of Wheatley's so let's add that to the count</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -1663,11 +1898,16 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>75 bottles of jim beam full bottle of makers mark full bottle of milagro reposado</t>
+          <t>22 cans of Yingling</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -1683,11 +1923,16 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.1</v>
+        <v>5</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>10 percent of a bottle of rumple mints 25 percent of a bottle of jagermeister</t>
+          <t>5 cans of athletic non-alcoholic beer</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -1703,11 +1948,16 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.75</v>
+        <v>12</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>75 percent of a bottle of rumple mints full bottle of jalapeno simple syrup</t>
+          <t>12 cans of Coors Light</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -1723,11 +1973,16 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.75</v>
+        <v>24</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>75 percent of a bottle of romano romana amaro full bottle of hendrix gin</t>
+          <t>24 cans of high noon</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -1743,11 +1998,16 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.85</v>
+        <v>2</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>walnut liqueur 85 percent of a bottle of tulamore dew 25 percent of a bottle of</t>
+          <t>2 bottles of Squealing Pig</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -1763,11 +2023,16 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>24</v>
+        <v>0.9</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>24 cans of myckelope ultra</t>
+          <t>half of a bottle of Pueblo Viejo 90% of a bottle of Yahweh 25% of a bottle of Eagle</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -1783,11 +2048,16 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>13</v>
+        <v>0.5</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>13 cans of greaton 30a gosey 24 more cans of myckelope ultra</t>
+          <t>Rare 10 year aged quarter of a bottle of E.H. Taylor half of a bottle of Parrot Bay white rum</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -1803,11 +2073,16 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>12</v>
+        <v>0.5</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>12 pack of pacifico two</t>
+          <t>then a half of a 750 milliliter bottle of</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -1823,11 +2098,16 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>12</v>
+        <v>0.2</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>12 cans of yingling</t>
+          <t>Grey Goose 20% of a bottle of Woodford half of a bottle of Jim Beam a full bottle of Mikters 80%</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -1843,11 +2123,16 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>20</v>
+        <v>0.25</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>20 cans of mom water got a high noon</t>
+          <t>of a bottle of Crown 25% of a bottle of Hendrick's Gin 90% of a bottle of Casamigos 25% of a bottle</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -1863,11 +2148,16 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0.75</v>
+        <v>0.85</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>full bottle of canoe ridge 75 percent of a bottle of canoe ridge full bottle of</t>
+          <t>of Milagro Reposado a full bottle of Milagro Silver 85% of a bottle of Blanton's 80% of a bottle</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -1883,11 +2173,16 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>144</v>
+        <v>0.98</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>12 bottle cases of 30a rose</t>
+          <t>of Caravella 98% of a bottle of Maker's Mark 80% of a bottle of Grand Gala 95% of a bottle</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -1903,11 +2198,16 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>144</v>
+        <v>0.1</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>12 bottle cases of 30a</t>
+          <t>of Bowles elderflower liqueur half of a bottle of Blue Curacao 10% of a bottle of Jack Daniels</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -1930,6 +2230,11 @@
           <t>27 bottles of marca de caseres so on top of the six that i just counted</t>
         </is>
       </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1950,6 +2255,11 @@
           <t>12 bottles of bloody mary mix</t>
         </is>
       </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1970,6 +2280,11 @@
           <t>10 bottles of strawberry puree</t>
         </is>
       </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1990,6 +2305,11 @@
           <t>24 pack of ginger beer</t>
         </is>
       </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2010,6 +2330,11 @@
           <t>24 pack of yingling</t>
         </is>
       </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2030,6 +2355,11 @@
           <t>12 packs of pacifico</t>
         </is>
       </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2050,6 +2380,11 @@
           <t>424 packs of make globe ultra</t>
         </is>
       </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2070,6 +2405,11 @@
           <t>12 pack of core's</t>
         </is>
       </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2090,6 +2430,11 @@
           <t>12 packs of corona extra cans</t>
         </is>
       </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2110,6 +2455,11 @@
           <t>12 packs of athletic</t>
         </is>
       </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2130,6 +2480,11 @@
           <t>10 bottles of blue curacao and the triple sec and the blue curacao both of those are the mr boston</t>
         </is>
       </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2150,6 +2505,11 @@
           <t>10 bottles of jaeger meister</t>
         </is>
       </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2170,6 +2530,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>back bar</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2190,6 +2555,11 @@
           <t>4 bottles of Scarpetta</t>
         </is>
       </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>storage</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2210,6 +2580,11 @@
           <t>eight bottles of scarpetta</t>
         </is>
       </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2230,6 +2605,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>back bar</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2243,11 +2623,16 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>one can of Miller Light</t>
+          <t>16 Miller lights</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -2267,7 +2652,12 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>one can of Coors Light</t>
+          <t>one can of Miller Light</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>inside bar</t>
         </is>
       </c>
     </row>
@@ -2283,11 +2673,16 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>16 Miller lights</t>
+          <t>one can of Coors Light</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>inside bar</t>
         </is>
       </c>
     </row>
@@ -2310,6 +2705,11 @@
           <t>half bottles of watermelon cocktail mix again that's four and a</t>
         </is>
       </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>back bar</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2330,6 +2730,11 @@
           <t>two bottles of grand marnier</t>
         </is>
       </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2350,6 +2755,11 @@
           <t>nine bottles of grand gala</t>
         </is>
       </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2363,11 +2773,16 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>caseres six more bottles of watermelon mixer half of a bottle of erradura ultra</t>
+          <t>full keg of Kona Big Wave all right now starting on the back bar we have three bottles of Tahin</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -2383,11 +2798,16 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>so in the walk-in there's one full keg of 38 beach blonde again those are half</t>
+          <t>two bottles of cream of coconut</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -2403,11 +2823,16 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>two cases of the fresh Victor's cucumber lime again</t>
+          <t>three cans of ginger beer</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -2423,11 +2848,16 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>two cases of those</t>
+          <t>one bottle of squealing pig Sauvignon Blanc</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -2443,11 +2873,16 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>0.2</v>
+        <v>4</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>the next place we're gonna count is the inside bar okay so inside bar we have four fifths of</t>
+          <t>four bottles of 30a chardonnay</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -2463,11 +2898,16 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>a bottle of Colonel E.H. Taylor small batch we have a quarter of a bottle of Pappas Pilar</t>
+          <t>one bottle of windstorm chardonnay</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -2483,11 +2923,16 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>one can of watermelon high noon</t>
+          <t>a half bottles of carter's lot rosé</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -2507,7 +2952,12 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>one can of Michelob Ultra</t>
+          <t>one bottle of sonoma coutrere wine white wine one more bottle of carter's lot rosé</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -2523,11 +2973,16 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>one can of Pacifico</t>
+          <t>two bottles of charles de fer prosecco</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -2543,11 +2998,16 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>one can of yingling</t>
+          <t>three bottles of marca de caseres</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -2567,7 +3027,12 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>one can of athletic upside Don</t>
+          <t>bottle of gray goose three full bottles of yave coconut tequila if i don't say you know if i just</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -2583,11 +3048,16 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>half of a bottle of the Eagle rare aged ten years because in the past we have had twelve</t>
+          <t>say bottles that means it's full if i don't specify the percentage</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -2603,11 +3073,16 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>0.75</v>
+        <v>0.33</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>this is the ten year three quarters of a bottle of red excuse me call it four fifths of a bottle</t>
+          <t>33 percent of a bottle of fireball two bottles of crown royal</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -2623,11 +3098,16 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>rum half of a bottle of Casamigos silver full bottle of grenadine half of a bottle of fireball</t>
+          <t>full bottle of jameson full bottle of sieta misterios mezcal full bottle of wheatleys</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -2643,11 +3123,16 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>90% of a bottle of farmers gin one full bottle of crop cucumber vodka quarter of a bottle of</t>
+          <t>full bottle of campesino silver rum half of a bottle of campesino aged rum</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -2663,11 +3148,16 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>7</v>
+        <v>0.33</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>7 cans of</t>
+          <t>33 percent of a bottle of nocello</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -2683,11 +3173,16 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>7 cans of Pacifico</t>
+          <t>four pack of mom waters</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -2703,11 +3198,16 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>6 cans of ginger beer</t>
+          <t>four packs of red bull</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -2723,11 +3223,16 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>0.5</v>
+        <v>6</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>half of a bottle of Myers aged rum a quarter of a bottle of Siete Mestadios mezcal a full bottle</t>
+          <t>six cans of red bull regular</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -2743,11 +3248,16 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>half bottle of crop cucumber vodka a</t>
+          <t>three cans of red bull low sugar</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -2763,11 +3273,16 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>half bottle of Wheatley's excuse me make that</t>
+          <t>one can of high noon</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -2783,11 +3298,16 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>full keg of Kona Big Wave all right now starting on the back bar we have three bottles of Tahin</t>
+          <t>the next place we're gonna count is the inside bar okay so inside bar we have four fifths of</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>inside bar</t>
         </is>
       </c>
     </row>
@@ -2803,11 +3323,16 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>2</v>
+        <v>0.25</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>two bottles of cream of coconut</t>
+          <t>a bottle of Colonel E.H. Taylor small batch we have a quarter of a bottle of Pappas Pilar</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>inside bar</t>
         </is>
       </c>
     </row>
@@ -2823,11 +3348,16 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>three cans of ginger beer</t>
+          <t>one can of watermelon high noon</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>inside bar</t>
         </is>
       </c>
     </row>
@@ -2847,7 +3377,12 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>one bottle of squealing pig Sauvignon Blanc</t>
+          <t>one can of Michelob Ultra</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>inside bar</t>
         </is>
       </c>
     </row>
@@ -2863,11 +3398,16 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>four bottles of 30a chardonnay</t>
+          <t>one can of Pacifico</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>inside bar</t>
         </is>
       </c>
     </row>
@@ -2887,7 +3427,12 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>one bottle of windstorm chardonnay</t>
+          <t>one can of yingling</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>inside bar</t>
         </is>
       </c>
     </row>
@@ -2903,11 +3448,16 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>a half bottles of carter's lot rosé</t>
+          <t>one can of athletic upside Don</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>inside bar</t>
         </is>
       </c>
     </row>
@@ -2923,11 +3473,16 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>one bottle of sonoma coutrere wine white wine one more bottle of carter's lot rosé</t>
+          <t>half of a bottle of the Eagle rare aged ten years because in the past we have had twelve</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>inside bar</t>
         </is>
       </c>
     </row>
@@ -2943,11 +3498,16 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>2</v>
+        <v>0.75</v>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>two bottles of charles de fer prosecco</t>
+          <t>this is the ten year three quarters of a bottle of red excuse me call it four fifths of a bottle</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>inside bar</t>
         </is>
       </c>
     </row>
@@ -2963,11 +3523,16 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>36</v>
+        <v>0.5</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>three bottles of marca de caseres</t>
+          <t>rum half of a bottle of Casamigos silver full bottle of grenadine half of a bottle of fireball</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>inside bar</t>
         </is>
       </c>
     </row>
@@ -2983,11 +3548,16 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>bottle of gray goose three full bottles of yave coconut tequila if i don't say you know if i just</t>
+          <t>90% of a bottle of farmers gin one full bottle of crop cucumber vodka quarter of a bottle of</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>inside bar</t>
         </is>
       </c>
     </row>
@@ -3003,11 +3573,16 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>say bottles that means it's full if i don't specify the percentage</t>
+          <t>7 cans of</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -3023,11 +3598,16 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>0.33</v>
+        <v>7</v>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>33 percent of a bottle of fireball two bottles of crown royal</t>
+          <t>7 cans of Pacifico</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -3043,11 +3623,16 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>full bottle of jameson full bottle of sieta misterios mezcal full bottle of wheatleys</t>
+          <t>6 cans of ginger beer</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -3067,7 +3652,12 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>full bottle of campesino silver rum half of a bottle of campesino aged rum</t>
+          <t>half of a bottle of Myers aged rum a quarter of a bottle of Siete Mestadios mezcal a full bottle</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -3083,11 +3673,16 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>33 percent of a bottle of nocello</t>
+          <t>half bottle of crop cucumber vodka a</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -3103,11 +3698,16 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>four pack of mom waters</t>
+          <t>half bottle of Wheatley's excuse me make that</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -3123,11 +3723,16 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>four packs of red bull</t>
+          <t>caseres six more bottles of watermelon mixer half of a bottle of erradura ultra</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>truck</t>
         </is>
       </c>
     </row>
@@ -3143,11 +3748,16 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>six cans of red bull regular</t>
+          <t>six bottle cases of crop organic cucumber vodka</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3777,12 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>three cans of red bull low sugar</t>
+          <t>three bottles of canoe ridge merlot</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3183,11 +3798,16 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>one can of high noon</t>
+          <t>four bottles of 30a chardonnay</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3203,11 +3823,16 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>six bottle cases of crop organic cucumber vodka</t>
+          <t>eight bottles of windstorm chardonnay</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3223,11 +3848,16 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>three bottles of canoe ridge merlot</t>
+          <t>two bottles of windstorm cabernet</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3243,11 +3873,16 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>four bottles of 30a chardonnay</t>
+          <t>six bottles of marca de caseres</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3263,11 +3898,16 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>eight bottles of windstorm chardonnay</t>
+          <t>nine bottles of stirring's watermelon cocktail mix</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3283,11 +3923,16 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>two bottles of windstorm cabernet</t>
+          <t>four packs of high</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3303,11 +3948,16 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>72</v>
+        <v>6</v>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>six bottles of marca de caseres</t>
+          <t>six packs or excuse me</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3323,11 +3973,16 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>nine bottles of stirring's watermelon cocktail mix</t>
+          <t>two cases of</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3343,11 +3998,16 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>four packs of high</t>
+          <t>six bottles of watermelon cocktail mix</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3363,11 +4023,16 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>six packs or excuse me</t>
+          <t>four packs i think i might have said something else but there's two</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3383,11 +4048,16 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>two cases of</t>
+          <t>four packs of red bull</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3403,11 +4073,16 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>six bottles of watermelon cocktail mix</t>
+          <t>nine bottles of yave coconut tequila</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3423,11 +4098,16 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>four packs i think i might have said something else but there's two</t>
+          <t>one bottle of casamigos</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3443,11 +4123,16 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>four packs of red bull</t>
+          <t>five bottles of caravela limoncello</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3463,11 +4148,16 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>nine bottles of yave coconut tequila</t>
+          <t>five bottles of campesino silver rum</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3483,11 +4173,16 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>one bottle of casamigos</t>
+          <t>five bottles of crown royal</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3503,11 +4198,16 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>five bottles of caravela limoncello</t>
+          <t>eight bottles of jack daniels</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3523,11 +4223,16 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>five bottles of campesino silver rum</t>
+          <t>two bottles of tia maria coffee liqueur</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3543,11 +4248,16 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>five bottles of crown royal</t>
+          <t>one bottle of nacello</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3563,11 +4273,16 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>8</v>
+        <v>0.5</v>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>eight bottles of jack daniels</t>
+          <t>so in the walk-in there's one full keg of 38 beach blonde again those are half</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>walk-in cooler</t>
         </is>
       </c>
     </row>
@@ -3583,11 +4298,16 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>two bottles of tia maria coffee liqueur</t>
+          <t>two cases of the fresh Victor's cucumber lime again</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>walk-in cooler</t>
         </is>
       </c>
     </row>
@@ -3603,11 +4323,16 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>one bottle of nacello</t>
+          <t>two cases of those</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>walk-in cooler</t>
         </is>
       </c>
     </row>
@@ -3623,11 +4348,16 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>six barrels three</t>
+          <t>8 bottles of mojito mix plus one more bottle of mojito mix</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -3643,11 +4373,16 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>six barrels of Paradise</t>
+          <t>one bottle of 30a rosé</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -3663,11 +4398,16 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>8 bottles of mojito mix plus one more bottle of mojito mix</t>
+          <t>apparol full bottle of bloody mary mix full bottle of jalapeno simple syrup</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -3683,11 +4423,16 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>one bottle of 30a rosé</t>
+          <t>eight bottles of mojito mix</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3703,11 +4448,16 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>apparol full bottle of bloody mary mix full bottle of jalapeno simple syrup</t>
+          <t>six bottles of angostura bitters i've got a</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3723,11 +4473,16 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>eight bottles of mojito mix</t>
+          <t>three bottles of woodford</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3747,7 +4502,12 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>six bottles of angostura bitters i've got a</t>
+          <t>six bottles of jamison</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>
@@ -3763,11 +4523,16 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>three bottles of woodford</t>
+          <t>six barrels three</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>walk-in cooler</t>
         </is>
       </c>
     </row>
@@ -3787,7 +4552,12 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>six bottles of jamison</t>
+          <t>six barrels of Paradise</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>walk-in cooler</t>
         </is>
       </c>
     </row>
@@ -3803,11 +4573,16 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>0.8</v>
+        <v>2</v>
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>Mark 80% of a bottle of Jim Beam 80% of a bottle of Tullamore Dew a third of a bottle of gray goose</t>
+          <t>two</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -3823,11 +4598,16 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>three-quarters of a bottle of Wheatley's vodka oh also in storage so let's add this to this</t>
+          <t>two full bottles of parrot bay white rum</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -3843,11 +4623,16 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>0.6</v>
+        <v>2</v>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>60% of a bottle of Wheatley's instead of a half</t>
+          <t>two</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -3870,6 +4655,11 @@
           <t>two</t>
         </is>
       </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>back bar</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -3883,11 +4673,16 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>two full bottles of parrot bay white rum</t>
+          <t>two</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -3910,6 +4705,11 @@
           <t>two</t>
         </is>
       </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>back bar</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -3923,11 +4723,16 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>2</v>
+        <v>0.8</v>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>two</t>
+          <t>Mark 80% of a bottle of Jim Beam 80% of a bottle of Tullamore Dew a third of a bottle of gray goose</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>inside bar</t>
         </is>
       </c>
     </row>
@@ -3943,11 +4748,16 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>2</v>
+        <v>0.25</v>
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>two</t>
+          <t>three-quarters of a bottle of Wheatley's vodka oh also in storage so let's add this to this</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -3963,11 +4773,16 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>2</v>
+        <v>0.6</v>
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>two</t>
+          <t>60% of a bottle of Wheatley's instead of a half</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -3990,6 +4805,11 @@
           <t>two</t>
         </is>
       </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -4010,6 +4830,11 @@
           <t>two</t>
         </is>
       </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -4030,6 +4855,11 @@
           <t>two bottles of parrot bay white rum</t>
         </is>
       </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -4050,6 +4880,11 @@
           <t>five bottles of bowls elderflower liqueur</t>
         </is>
       </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -4070,6 +4905,11 @@
           <t>one bottle of tolamore dew</t>
         </is>
       </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -4087,7 +4927,12 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>of a bottle of Tanqueray half of a bottle of Milagro Reposado half of a bottle of Parrot</t>
+          <t>half bottles of</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -4103,11 +4948,16 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>half of a bottle of Tanqueray</t>
+          <t>five bottles of</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -4123,11 +4973,16 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>half of a bottle of Jameson half of a keg of Paradise Park a full keg of Stella Artois</t>
+          <t>apparol full bottle of farmers gin</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -4143,11 +4998,16 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>half bottles of</t>
+          <t>got one full bottle of the shaker red blend</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>back bar</t>
         </is>
       </c>
     </row>
@@ -4163,11 +5023,16 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>five bottles of</t>
+          <t>of a bottle of Tanqueray half of a bottle of Milagro Reposado half of a bottle of Parrot</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>inside bar</t>
         </is>
       </c>
     </row>
@@ -4183,11 +5048,16 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>apparol full bottle of farmers gin</t>
+          <t>half of a bottle of Tanqueray</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -4203,11 +5073,16 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>got one full bottle of the shaker red blend</t>
+          <t>half of a bottle of Jameson half of a keg of Paradise Park a full keg of Stella Artois</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>storage</t>
         </is>
       </c>
     </row>
@@ -4230,6 +5105,11 @@
           <t>nine bottles of the shaker red blend</t>
         </is>
       </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -4250,6 +5130,11 @@
           <t>one bottle of eridura reposado</t>
         </is>
       </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -4270,6 +5155,11 @@
           <t>four bottles of blue agave i have four</t>
         </is>
       </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -4290,6 +5180,11 @@
           <t>seven bottles of parrot bay</t>
         </is>
       </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -4310,6 +5205,11 @@
           <t>nine bottles of rumple mints</t>
         </is>
       </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -4330,6 +5230,11 @@
           <t>seven bottles of romana amaro</t>
         </is>
       </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -4350,6 +5255,11 @@
           <t>three bottles of maker's mark</t>
         </is>
       </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -4370,6 +5280,11 @@
           <t>five bottles of</t>
         </is>
       </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -4390,6 +5305,11 @@
           <t>one bottle of jaeger</t>
         </is>
       </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -4410,6 +5330,11 @@
           <t>one bottle of fireball</t>
         </is>
       </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -4430,6 +5355,11 @@
           <t>eight bottles of tanker a</t>
         </is>
       </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -4450,6 +5380,11 @@
           <t>nine bottles of apparel</t>
         </is>
       </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>upstairs</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -4468,6 +5403,11 @@
       <c r="D188" t="inlineStr">
         <is>
           <t>one</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>upstairs</t>
         </is>
       </c>
     </row>

</xml_diff>